<commit_message>
Phân công lại cho mọi người nhé
</commit_message>
<xml_diff>
--- a/Phân_Công.xlsx
+++ b/Phân_Công.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
   <si>
     <t>STT</t>
   </si>
@@ -48,9 +48,6 @@
     <t>9h-10h</t>
   </si>
   <si>
-    <t>10h-11h</t>
-  </si>
-  <si>
     <t>Xây dựng module hướng dẫn sử dụng phần mềm (menu Help, F1) chi tiết đến từng chức năng</t>
   </si>
   <si>
@@ -156,10 +153,10 @@
     <t>Leader : maingocle</t>
   </si>
   <si>
-    <t>10h-12h</t>
-  </si>
-  <si>
     <t>5h-6h</t>
+  </si>
+  <si>
+    <t>7h-8h</t>
   </si>
 </sst>
 </file>
@@ -602,7 +599,7 @@
   <dimension ref="A1:H19"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +610,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -655,7 +652,7 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
@@ -664,14 +661,14 @@
     <row r="5" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>6</v>
@@ -680,14 +677,14 @@
     <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="D6" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>8</v>
@@ -696,78 +693,78 @@
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>9</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H11" s="7" t="s">
         <v>45</v>
@@ -776,14 +773,14 @@
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H12" s="7" t="s">
         <v>45</v>
@@ -792,14 +789,14 @@
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H13" s="7" t="s">
         <v>45</v>
@@ -808,14 +805,14 @@
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H14" s="7" t="s">
         <v>45</v>
@@ -824,62 +821,62 @@
     <row r="15" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="4" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
     </row>
     <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>8</v>
@@ -888,14 +885,14 @@
     <row r="19" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>8</v>

</xml_diff>

<commit_message>
mình sửa lại 1 chút chỗ phân công mọi người nhé
</commit_message>
<xml_diff>
--- a/Phân_Công.xlsx
+++ b/Phân_Công.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="45">
   <si>
     <t>STT</t>
   </si>
@@ -67,9 +67,6 @@
   </si>
   <si>
     <t>Huyền</t>
-  </si>
-  <si>
-    <t>Ngọc</t>
   </si>
   <si>
     <t>Lệ</t>
@@ -598,8 +595,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -610,7 +607,7 @@
   <sheetData>
     <row r="1" spans="1:8" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="9" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B1" s="9"/>
       <c r="C1" s="9"/>
@@ -652,7 +649,7 @@
       </c>
       <c r="D4" s="2"/>
       <c r="E4" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="F4" s="3"/>
       <c r="G4" s="4"/>
@@ -661,14 +658,14 @@
     <row r="5" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C5" s="1"/>
       <c r="D5" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="F5" s="3"/>
       <c r="G5" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H5" s="7" t="s">
         <v>6</v>
@@ -677,14 +674,14 @@
     <row r="6" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C6" s="1"/>
       <c r="D6" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E6" s="6" t="s">
         <v>7</v>
       </c>
       <c r="F6" s="3"/>
       <c r="G6" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H6" s="7" t="s">
         <v>8</v>
@@ -693,142 +690,142 @@
     <row r="7" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C7" s="1"/>
       <c r="D7" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F7" s="3"/>
       <c r="G7" s="4" t="s">
         <v>14</v>
       </c>
       <c r="H7" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C8" s="1"/>
       <c r="D8" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F8" s="3"/>
       <c r="G8" s="4" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H8" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C9" s="1"/>
       <c r="D9" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="F9" s="3"/>
       <c r="G9" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H9" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="10" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C10" s="1"/>
       <c r="D10" s="2" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F10" s="3"/>
       <c r="G10" s="4" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C11" s="1"/>
       <c r="D11" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="3"/>
       <c r="G11" s="4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="12" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C12" s="1"/>
       <c r="D12" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="H12" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="13" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C13" s="1"/>
       <c r="D13" s="2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="H13" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C14" s="1"/>
       <c r="D14" s="2" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F14" s="3"/>
       <c r="G14" s="4" t="s">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="H14" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C15" s="1"/>
       <c r="D15" s="2" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F15" s="3"/>
       <c r="G15" s="4" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="H15" s="7" t="s">
         <v>6</v>
@@ -837,46 +834,46 @@
     <row r="16" spans="1:8" ht="47.25" x14ac:dyDescent="0.25">
       <c r="C16" s="1"/>
       <c r="D16" s="2" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E16" s="6" t="s">
         <v>9</v>
       </c>
       <c r="F16" s="3"/>
       <c r="G16" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H16" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="17" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C17" s="1"/>
       <c r="D17" s="2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E17" s="6" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="3"/>
       <c r="G17" s="4" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H17" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="18" spans="3:8" ht="31.5" x14ac:dyDescent="0.25">
       <c r="C18" s="1"/>
       <c r="D18" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="E18" s="6" t="s">
         <v>11</v>
       </c>
       <c r="F18" s="3"/>
       <c r="G18" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H18" s="7" t="s">
         <v>8</v>
@@ -885,14 +882,14 @@
     <row r="19" spans="3:8" ht="15.75" x14ac:dyDescent="0.25">
       <c r="C19" s="1"/>
       <c r="D19" s="2" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E19" s="6" t="s">
         <v>12</v>
       </c>
       <c r="F19" s="3"/>
       <c r="G19" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H19" s="7" t="s">
         <v>8</v>

</xml_diff>